<commit_message>
implementacion de codigo oferta, vista previa puntos oferta,tooltips botones, quitar puntos ai,ao,bi,bo de oferta, borrar modificar producto,cambiar nombre de pagina,nit en la oferta
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="TAB 01" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Supervisor" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TAB 02" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TAB 03" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Supervisor" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -500,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +533,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CENTAURO</t>
+          <t>SAN MARTIN</t>
         </is>
       </c>
     </row>
@@ -555,20 +557,20 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>LG BECON CONTROLLER</t>
+          <t>JCI FACILITY EXPLORER</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -583,16 +585,16 @@
     </row>
     <row r="5">
       <c r="C5" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="F5" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -610,13 +612,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -711,7 +713,7 @@
     <row r="9">
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>UMA 01</t>
+          <t>VENT 01</t>
         </is>
       </c>
       <c r="K9" s="3" t="inlineStr">
@@ -721,23 +723,26 @@
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>VDQ-00QA2</t>
+          <t>F4-CGM09090</t>
         </is>
       </c>
       <c r="M9" s="8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N9" s="8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O9" s="8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P9" s="8" t="n">
         <v>3</v>
       </c>
+      <c r="Q9" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R9" s="9" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -746,16 +751,41 @@
       </c>
       <c r="B10" s="10" t="inlineStr">
         <is>
-          <t>FDFD</t>
-        </is>
-      </c>
-      <c r="E10" s="11" t="n">
+          <t>EST VENT 01</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="12" t="inlineStr">
         <is>
-          <t>AO - T&amp;S</t>
-        </is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>FX-PCX4711-0</t>
+        </is>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" s="9" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -764,39 +794,16 @@
       </c>
       <c r="B11" s="10" t="inlineStr">
         <is>
-          <t>FDFD</t>
-        </is>
-      </c>
-      <c r="D11" s="11" t="n">
-        <v>1</v>
+          <t>TEM SUM VENT 01</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>2</v>
       </c>
       <c r="H11" s="12" t="inlineStr">
         <is>
-          <t>BI - T&amp;S</t>
-        </is>
-      </c>
-      <c r="L11" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
-        </is>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="N11" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="O11" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="P11" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="9" t="n">
-        <v>16</v>
+          <t>EHD110-800 - SCHNEIDER</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -805,87 +812,357 @@
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>FDFD</t>
-        </is>
-      </c>
-      <c r="F12" s="11" t="n">
+          <t>HUM VENT 01</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="12" t="inlineStr">
         <is>
-          <t>BO - T&amp;S</t>
+          <t>AQD-BBBE - SENVA</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
         <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>STAR/STOP VENT 01</t>
+        </is>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
           <t>PUNTOS PROYECTADOS</t>
         </is>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="N12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="3" t="n">
+      <c r="P13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="R12" s="9" t="n">
+      <c r="R13" s="9" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>VENT 02</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="R14" s="9" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>TEM SUM VENT 02</t>
+        </is>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="12" t="inlineStr">
+        <is>
+          <t>EHD110-800 - SCHNEIDER</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>EST VENT 02</t>
+        </is>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="L13" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M13" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="N13" s="4" t="n">
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>STAR/STOP VENT 02</t>
+        </is>
+      </c>
+      <c r="F17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+      <c r="K17" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L17" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>HUM VENT 02</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+      <c r="K18" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="13" t="inlineStr">
+        <is>
+          <t>TR75VA004</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>VENT 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>TEM SUM VENT 03</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>EHD110-800 - SCHNEIDER</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>EST VENT 03</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="O13" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="P13" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="9" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16">
-      <c r="K16" s="1" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="L16" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="K17" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="13" t="inlineStr">
-        <is>
-          <t>TR40VA004</t>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>STAR/STOP VENT 03</t>
+        </is>
+      </c>
+      <c r="F22" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>HUM VENT 03</t>
+        </is>
+      </c>
+      <c r="C23" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>VENT 04</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>TEM SUM VENT 03</t>
+        </is>
+      </c>
+      <c r="C25" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="12" t="inlineStr">
+        <is>
+          <t>EHD110-800 - SCHNEIDER</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>EST VENT 01</t>
+        </is>
+      </c>
+      <c r="D26" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>STAR/STOP VENT 03</t>
+        </is>
+      </c>
+      <c r="F27" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>HUM VENT 03</t>
+        </is>
+      </c>
+      <c r="C28" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
         </is>
       </c>
     </row>
@@ -895,6 +1172,1117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="2" customWidth="1" min="9" max="9"/>
+    <col width="2" customWidth="1" min="10" max="10"/>
+    <col width="5" customWidth="1" min="11" max="11"/>
+    <col width="32" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>PROYECTO</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>SAN MARTIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SISTEMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TAB 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SOLUCIÓN</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>JCI FACILITY EXPLORER</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>NOTAS / TIPO DE SENSOR / ACTUADOR</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>CONTROLADOR / EXPANSIÓN</t>
+        </is>
+      </c>
+      <c r="M8" s="5" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="O8" s="5" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="P8" s="5" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="Q8" s="5" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="R8" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>CHILLER 01</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>F4-CGM04060</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>START/STOP CHILLER 01</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>APER VAL 01</t>
+        </is>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
+        <is>
+          <t>AO - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>FEEDBACK VALV 01</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
+        <is>
+          <t>AI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>CHILLER 02</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>START/STOP CHILLER 02</t>
+        </is>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>APER VAL 02</t>
+        </is>
+      </c>
+      <c r="E15" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="inlineStr">
+        <is>
+          <t>AO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>FEEDBACK VALV 02</t>
+        </is>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12" t="inlineStr">
+        <is>
+          <t>AI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>CHILLER 03</t>
+        </is>
+      </c>
+      <c r="K17" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13" t="inlineStr">
+        <is>
+          <t>TR40VA004</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>START/STOP CHILLER 03</t>
+        </is>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>APER VAL 03</t>
+        </is>
+      </c>
+      <c r="E19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12" t="inlineStr">
+        <is>
+          <t>AO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>FEEDBACK VALV 03</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>AI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="2" customWidth="1" min="9" max="9"/>
+    <col width="2" customWidth="1" min="10" max="10"/>
+    <col width="5" customWidth="1" min="11" max="11"/>
+    <col width="32" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>PROYECTO</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>SAN MARTIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SISTEMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TAB 03</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SOLUCIÓN</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>JCI FACILITY EXPLORER</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>NOTAS / TIPO DE SENSOR / ACTUADOR</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>CONTROLADOR / EXPANSIÓN</t>
+        </is>
+      </c>
+      <c r="M8" s="5" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="O8" s="5" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="P8" s="5" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="Q8" s="5" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="R8" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>UMA 02</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>F4-CGM04060</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>SENSOR CO2 UMA 02</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>FX-PCX4711-0</t>
+        </is>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" s="9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>TE RET UMA 02</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>EST DPS UMA 01</t>
+        </is>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>EST-MERV8 UMA 02</t>
+        </is>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>CAUDAL FLU-UMA01</t>
+        </is>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="R14" s="9" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>TE SUMINISTRO UMA 02</t>
+        </is>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>EST MERV14 UMA 02</t>
+        </is>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>K1 ON/OFF UMA 02</t>
+        </is>
+      </c>
+      <c r="F17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+      <c r="K17" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L17" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>EST MOTOR 1</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K18" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="13" t="inlineStr">
+        <is>
+          <t>TR75VA004</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>EST MOTOR 2</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>EST MOTOR 3</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>VDF UMA 02</t>
+        </is>
+      </c>
+      <c r="E21" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="inlineStr">
+        <is>
+          <t>AO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>DAMPER MEZCLA UMA 02</t>
+        </is>
+      </c>
+      <c r="E22" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12" t="inlineStr">
+        <is>
+          <t>AO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -938,12 +2326,12 @@
     <row r="3">
       <c r="B3" s="14" t="inlineStr">
         <is>
-          <t>SNE10500</t>
+          <t>SNE1100</t>
         </is>
       </c>
       <c r="C3" s="14" t="inlineStr">
         <is>
-          <t>MODULO SUPERVISOR METASYS (SNE10500); Máximo de integraciones permitidas (60);1 Ethernet port ; 1 RS-485 ports; 2 USB ports</t>
+          <t>MODULO SUPERVISOR METASYS (SNE11000); Máximo de integraciones permitidas (150);1 Ethernet port ; 1 RS-485 ports; 2 USB ports</t>
         </is>
       </c>
       <c r="F3" s="14" t="n">

</xml_diff>

<commit_message>
sistema de navegacion arbol
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -126,10 +126,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -560,16 +560,16 @@
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -584,10 +584,10 @@
     </row>
     <row r="5">
       <c r="C5" s="3" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>
@@ -611,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>2</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>10</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -722,26 +722,23 @@
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>F4-CGM09090</t>
+          <t>F4-CGM04060</t>
         </is>
       </c>
       <c r="M9" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8" t="n">
         <v>2</v>
-      </c>
-      <c r="O9" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P9" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="Q9" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R9" s="9" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -753,38 +750,10 @@
           <t>EST VENT 01</t>
         </is>
       </c>
-      <c r="D10" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="12" t="inlineStr">
+      <c r="H10" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
         </is>
-      </c>
-      <c r="K10" s="3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="L10" s="7" t="inlineStr">
-        <is>
-          <t>FX-PCX4711-0</t>
-        </is>
-      </c>
-      <c r="M10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="N10" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P10" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="R10" s="9" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -796,13 +765,33 @@
           <t>TEM SUM VENT 01</t>
         </is>
       </c>
-      <c r="C11" s="11" t="n">
+      <c r="H11" s="11" t="inlineStr">
+        <is>
+          <t>EHD110-800 - SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="12" t="inlineStr">
-        <is>
-          <t>EHD110-800 - SCHNEIDER</t>
-        </is>
+      <c r="Q11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -814,36 +803,33 @@
           <t>HUM VENT 01</t>
         </is>
       </c>
-      <c r="C12" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12" t="inlineStr">
+      <c r="H12" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
         <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+          <t>PUNTOS PROYECTADOS</t>
         </is>
       </c>
       <c r="M12" s="3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="N12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" s="9" t="n">
         <v>4</v>
-      </c>
-      <c r="O12" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="P12" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q12" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="R12" s="9" t="n">
-        <v>33</v>
       </c>
     </row>
     <row r="13">
@@ -855,36 +841,36 @@
           <t>STAR/STOP VENT 01</t>
         </is>
       </c>
-      <c r="F13" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12" t="inlineStr">
+      <c r="F13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11" t="inlineStr">
         <is>
           <t>CKIT-VMD1B-C24A - VERIS</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
         <is>
-          <t>PUNTOS PROYECTADOS</t>
-        </is>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="O13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="3" t="n">
-        <v>0</v>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="R13" s="9" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -893,29 +879,6 @@
           <t>VENT 02</t>
         </is>
       </c>
-      <c r="L14" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="P14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="R14" s="9" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
@@ -926,10 +889,7 @@
           <t>TEM SUM VENT 02</t>
         </is>
       </c>
-      <c r="C15" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="12" t="inlineStr">
+      <c r="H15" s="11" t="inlineStr">
         <is>
           <t>EHD110-800 - SCHNEIDER</t>
         </is>
@@ -944,12 +904,19 @@
           <t>EST VENT 02</t>
         </is>
       </c>
-      <c r="D16" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="12" t="inlineStr">
+      <c r="H16" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
         </is>
       </c>
     </row>
@@ -962,22 +929,20 @@
           <t>STAR/STOP VENT 02</t>
         </is>
       </c>
-      <c r="F17" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="12" t="inlineStr">
+      <c r="F17" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="11" t="inlineStr">
         <is>
           <t>CKIT-VMD1B-C24A - VERIS</t>
         </is>
       </c>
-      <c r="K17" s="1" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="L17" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
+      <c r="K17" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13" t="inlineStr">
+        <is>
+          <t>TR40VA004</t>
         </is>
       </c>
     </row>
@@ -990,20 +955,9 @@
           <t>HUM VENT 02</t>
         </is>
       </c>
-      <c r="C18" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="12" t="inlineStr">
+      <c r="H18" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
-        </is>
-      </c>
-      <c r="K18" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="13" t="inlineStr">
-        <is>
-          <t>TR75VA004</t>
         </is>
       </c>
     </row>
@@ -1023,10 +977,7 @@
           <t>TEM SUM VENT 03</t>
         </is>
       </c>
-      <c r="C20" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="H20" s="12" t="inlineStr">
+      <c r="H20" s="11" t="inlineStr">
         <is>
           <t>EHD110-800 - SCHNEIDER</t>
         </is>
@@ -1041,10 +992,7 @@
           <t>EST VENT 03</t>
         </is>
       </c>
-      <c r="D21" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="12" t="inlineStr">
+      <c r="H21" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
         </is>
@@ -1059,10 +1007,10 @@
           <t>STAR/STOP VENT 03</t>
         </is>
       </c>
-      <c r="F22" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="12" t="inlineStr">
+      <c r="F22" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="11" t="inlineStr">
         <is>
           <t>CKIT-VMD1B-C24A - VERIS</t>
         </is>
@@ -1077,10 +1025,7 @@
           <t>HUM VENT 03</t>
         </is>
       </c>
-      <c r="C23" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="12" t="inlineStr">
+      <c r="H23" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
@@ -1102,10 +1047,7 @@
           <t>TEM SUM VENT 03</t>
         </is>
       </c>
-      <c r="C25" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="H25" s="12" t="inlineStr">
+      <c r="H25" s="11" t="inlineStr">
         <is>
           <t>EHD110-800 - SCHNEIDER</t>
         </is>
@@ -1120,10 +1062,7 @@
           <t>EST VENT 01</t>
         </is>
       </c>
-      <c r="D26" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="12" t="inlineStr">
+      <c r="H26" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
         </is>
@@ -1138,10 +1077,10 @@
           <t>STAR/STOP VENT 03</t>
         </is>
       </c>
-      <c r="F27" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="12" t="inlineStr">
+      <c r="F27" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="11" t="inlineStr">
         <is>
           <t>CKIT-VMD1B-C24A - VERIS</t>
         </is>
@@ -1156,10 +1095,7 @@
           <t>HUM VENT 03</t>
         </is>
       </c>
-      <c r="C28" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="12" t="inlineStr">
+      <c r="H28" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
@@ -1235,16 +1171,16 @@
         </is>
       </c>
       <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>4</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>8</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -1259,10 +1195,10 @@
     </row>
     <row r="5">
       <c r="C5" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>2</v>
@@ -1286,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -1425,38 +1361,10 @@
           <t>SENSOR CO2 UMA 02</t>
         </is>
       </c>
-      <c r="C10" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="12" t="inlineStr">
+      <c r="H10" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
-      </c>
-      <c r="K10" s="3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="L10" s="7" t="inlineStr">
-        <is>
-          <t>FX-PCX4711-0</t>
-        </is>
-      </c>
-      <c r="M10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="N10" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P10" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="R10" s="9" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -1468,13 +1376,33 @@
           <t>TE RET UMA 02</t>
         </is>
       </c>
-      <c r="C11" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="12" t="inlineStr">
+      <c r="H11" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1486,36 +1414,33 @@
           <t>EST DPS UMA 01</t>
         </is>
       </c>
-      <c r="D12" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12" t="inlineStr">
+      <c r="H12" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
         <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+          <t>PUNTOS PROYECTADOS</t>
         </is>
       </c>
       <c r="M12" s="3" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R12" s="9" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -1527,36 +1452,33 @@
           <t>EST-MERV8 UMA 02</t>
         </is>
       </c>
-      <c r="D13" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12" t="inlineStr">
+      <c r="H13" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
         <is>
-          <t>PUNTOS PROYECTADOS</t>
-        </is>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="O13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="3" t="n">
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4" t="n">
         <v>2</v>
       </c>
       <c r="R13" s="9" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -1568,36 +1490,10 @@
           <t>CAUDAL FLU-UMA01</t>
         </is>
       </c>
-      <c r="C14" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="12" t="inlineStr">
+      <c r="H14" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
-      </c>
-      <c r="L14" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="R14" s="9" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -1609,10 +1505,7 @@
           <t>TE SUMINISTRO UMA 02</t>
         </is>
       </c>
-      <c r="C15" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="12" t="inlineStr">
+      <c r="H15" s="11" t="inlineStr">
         <is>
           <t>AQD-BBBE - SENVA</t>
         </is>
@@ -1627,12 +1520,19 @@
           <t>EST MERV14 UMA 02</t>
         </is>
       </c>
-      <c r="D16" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="12" t="inlineStr">
+      <c r="H16" s="11" t="inlineStr">
         <is>
           <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
         </is>
       </c>
     </row>
@@ -1645,22 +1545,20 @@
           <t>K1 ON/OFF UMA 02</t>
         </is>
       </c>
-      <c r="F17" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="12" t="inlineStr">
+      <c r="F17" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="11" t="inlineStr">
         <is>
           <t>CKIT-VMD1B-C24A - VERIS</t>
         </is>
       </c>
-      <c r="K17" s="1" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="L17" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
+      <c r="K17" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13" t="inlineStr">
+        <is>
+          <t>TR40VA004</t>
         </is>
       </c>
     </row>
@@ -1673,20 +1571,12 @@
           <t>EST MOTOR 1</t>
         </is>
       </c>
-      <c r="D18" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="12" t="inlineStr">
+      <c r="D18" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="11" t="inlineStr">
         <is>
           <t>BI - T&amp;S</t>
-        </is>
-      </c>
-      <c r="K18" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="13" t="inlineStr">
-        <is>
-          <t>TR75VA004</t>
         </is>
       </c>
     </row>
@@ -1699,10 +1589,10 @@
           <t>EST MOTOR 2</t>
         </is>
       </c>
-      <c r="D19" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="12" t="inlineStr">
+      <c r="D19" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11" t="inlineStr">
         <is>
           <t>BI - T&amp;S</t>
         </is>
@@ -1717,10 +1607,10 @@
           <t>EST MOTOR 3</t>
         </is>
       </c>
-      <c r="D20" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="12" t="inlineStr">
+      <c r="D20" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11" t="inlineStr">
         <is>
           <t>BI - T&amp;S</t>
         </is>
@@ -1735,10 +1625,10 @@
           <t>VDF UMA 02</t>
         </is>
       </c>
-      <c r="E21" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="12" t="inlineStr">
+      <c r="E21" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11" t="inlineStr">
         <is>
           <t>AO - T&amp;S</t>
         </is>
@@ -1753,10 +1643,10 @@
           <t>DAMPER MEZCLA UMA 02</t>
         </is>
       </c>
-      <c r="E22" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="12" t="inlineStr">
+      <c r="E22" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="11" t="inlineStr">
         <is>
           <t>AO - T&amp;S</t>
         </is>

</xml_diff>

<commit_message>
mejora de carga de item de formato svg, vista editar oferta.
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -1,8 +1,24 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="TAB CONT 01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TAB CONT 02" sheetId="2" state="visible" r:id="rId2"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -10,16 +26,62 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00000000"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+    </font>
+    <font/>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DAD7D7"/>
+        <bgColor rgb="00DAD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8CCE4"/>
+        <bgColor rgb="00B8CCE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FEFE7A"/>
+        <bgColor rgb="00FEFE7A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00808080"/>
+        <bgColor rgb="00808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090D473"/>
+        <bgColor rgb="0090D473"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -27,12 +89,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -390,4 +489,836 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="2" customWidth="1" min="9" max="9"/>
+    <col width="2" customWidth="1" min="10" max="10"/>
+    <col width="5" customWidth="1" min="11" max="11"/>
+    <col width="32" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>PROYECTO</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>PROYECTO 100</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SISTEMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TAB CONT 01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SOLUCIÓN</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>LG BECON CONTROLLER</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>NOTAS / TIPO DE SENSOR / ACTUADOR</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>CONTROLADOR / EXPANSIÓN</t>
+        </is>
+      </c>
+      <c r="M8" s="5" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="O8" s="5" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="P8" s="5" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="Q8" s="5" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="R8" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>VENT 01</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>VDQ-00QA2</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" s="9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>RLY KIT-VMD1B-C24A</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>CONTROL DE PRESIÓN DIFERENCIAL</t>
+        </is>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>CONDUCTO DE TEMPERATURA DE HUMEDAD</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
+        <is>
+          <t>HT1D - SENVA</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16">
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="K17" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13" t="inlineStr">
+        <is>
+          <t>TR40VA004</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="2" customWidth="1" min="9" max="9"/>
+    <col width="2" customWidth="1" min="10" max="10"/>
+    <col width="5" customWidth="1" min="11" max="11"/>
+    <col width="32" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>PROYECTO</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>PROYECTO 100</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SISTEMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TAB CONT 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SOLUCIÓN</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>LG BECON CONTROLLER</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>NOTAS / TIPO DE SENSOR / ACTUADOR</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>CONTROLADOR / EXPANSIÓN</t>
+        </is>
+      </c>
+      <c r="M8" s="5" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="O8" s="5" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="P8" s="5" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="Q8" s="5" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="R8" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>VENT 01</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>VDQ-00QA2</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" s="9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>CONTROL DE PRESIÓN DIFERENCIAL</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>RLY KIT-VMD1B-C24A</t>
+        </is>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>SENSOR DE TEMPERATURA DEL CONDUCTO</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>EHD110-800 - SCHNEIDER</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16">
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="K17" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13" t="inlineStr">
+        <is>
+          <t>TR40VA004</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formato celular, descargar y cargar categorias.
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TAB 01" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TAB  02" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TAB CONT 01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Supervisor" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,8 +33,17 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+    </font>
+    <font/>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -45,6 +54,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="00DAD7D7"/>
         <bgColor rgb="00DAD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8CCE4"/>
+        <bgColor rgb="00B8CCE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FEFE7A"/>
+        <bgColor rgb="00FEFE7A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00808080"/>
+        <bgColor rgb="00808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -72,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -83,17 +110,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +531,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>PADMITOS</t>
+          <t>CFP2</t>
         </is>
       </c>
     </row>
@@ -503,7 +543,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>TAB 01</t>
+          <t>TAB CONT 01</t>
         </is>
       </c>
     </row>
@@ -515,44 +555,44 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>LG BECON CONTROLLER</t>
+          <t>JCI FACILITY EXPLORER</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>&lt;==</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
+      <c r="F5" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -570,13 +610,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -668,103 +708,334 @@
         </is>
       </c>
     </row>
-    <row r="9"/>
+    <row r="9">
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>VENT 01</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>F4-CGM04060</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
     <row r="10">
-      <c r="L10" s="1" t="inlineStr">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>CONTROL DE PRESIÓN DIFERENCIAL SWITCH</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>FX-PCX4711-0</t>
+        </is>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" s="9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>CONDUCTO DE TEMPERATURA DE HUMEDAD</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
+        <is>
+          <t>HT1D - SENVA</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
         <is>
           <t>PUNTOS DISPONIBLES EN CONTROLES</t>
         </is>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M12" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="P12" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>START/STOP VENT 01</t>
+        </is>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="3" t="n">
+      <c r="P13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="P10" s="3" t="n">
+      <c r="R13" s="9" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>PARO DE EMERGANCIA</t>
+        </is>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="3" t="n">
+      <c r="O14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R10" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="L11" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS PROYECTADOS</t>
-        </is>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="L12" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14"/>
+      <c r="P14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="R14" s="9" t="n">
+        <v>13</v>
+      </c>
+    </row>
     <row r="15">
-      <c r="K15" s="1" t="inlineStr">
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>VENT 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
+        </is>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12" t="inlineStr">
+        <is>
+          <t>AQD-BBBE - SENVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>CONTROL DE PRESIÓN DIFERENCIAL SWITCH</t>
+        </is>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12" t="inlineStr">
+        <is>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+      <c r="K17" s="1" t="inlineStr">
         <is>
           <t>CANT</t>
         </is>
       </c>
-      <c r="L15" s="1" t="inlineStr">
+      <c r="L17" s="1" t="inlineStr">
         <is>
           <t>ACCESORIO</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="K16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="7" t="inlineStr">
-        <is>
-          <t>TR40VA004</t>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>CONDUCTO DE TEMPERATURA DE HUMEDAD</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>HT1D - SENVA</t>
+        </is>
+      </c>
+      <c r="K18" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="13" t="inlineStr">
+        <is>
+          <t>TR75VA004</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>START/STOP VENT 02</t>
+        </is>
+      </c>
+      <c r="F19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A - VERIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>PARO DE EMERGANCIA</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
@@ -779,7 +1050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,303 +1058,98 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="5" customWidth="1" min="3" max="3"/>
-    <col width="5" customWidth="1" min="4" max="4"/>
-    <col width="5" customWidth="1" min="5" max="5"/>
-    <col width="5" customWidth="1" min="6" max="6"/>
-    <col width="4" customWidth="1" min="7" max="7"/>
-    <col width="50" customWidth="1" min="8" max="8"/>
-    <col width="2" customWidth="1" min="9" max="9"/>
-    <col width="2" customWidth="1" min="10" max="10"/>
-    <col width="5" customWidth="1" min="11" max="11"/>
-    <col width="32" customWidth="1" min="12" max="12"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="100" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>PROYECTO</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>PADMITOS</t>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>SUPERVISOR</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>SISTEMA</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>TAB  02</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>SOLUCIÓN</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>LG BECON CONTROLLER</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>&lt;==</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+      <c r="B3" s="14" t="inlineStr">
+        <is>
+          <t>FX80</t>
+        </is>
+      </c>
+      <c r="C3" s="14" t="inlineStr">
+        <is>
+          <t>MODULO SUPERVISOR JC FX80</t>
+        </is>
+      </c>
+      <c r="F3" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14" t="inlineStr">
+        <is>
+          <t>TR40VA004</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>&lt;==</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS PROYECTADOS</t>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>LICENCIA</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>&lt;==</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-    </row>
-    <row r="7"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>FX-SC8BASE-0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Controlador de supervisión FX80 y tarjeta micro Secure Digital (SD)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FX-SC8CL005-0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Licencia de dispositivo central del controlador de supervisión FX80; 5 dispositivos de campo; 250 puntos</t>
+        </is>
+      </c>
+    </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>ED</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="inlineStr">
-        <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="G8" s="1" t="n"/>
-      <c r="H8" s="1" t="inlineStr">
-        <is>
-          <t>NOTAS / TIPO DE SENSOR / ACTUADOR</t>
-        </is>
-      </c>
-      <c r="K8" s="5" t="inlineStr">
-        <is>
-          <t>TIPO</t>
-        </is>
-      </c>
-      <c r="L8" s="5" t="inlineStr">
-        <is>
-          <t>CONTROLADOR / EXPANSIÓN</t>
-        </is>
-      </c>
-      <c r="M8" s="5" t="inlineStr">
-        <is>
-          <t>EU</t>
-        </is>
-      </c>
-      <c r="N8" s="5" t="inlineStr">
-        <is>
-          <t>ED</t>
-        </is>
-      </c>
-      <c r="O8" s="5" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="P8" s="5" t="inlineStr">
-        <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="Q8" s="5" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="R8" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="9"/>
-    <row r="10">
-      <c r="L10" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
-        </is>
-      </c>
-      <c r="M10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="L11" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS PROYECTADOS</t>
-        </is>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="L12" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15">
-      <c r="K15" s="1" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="L15" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="K16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="7" t="inlineStr">
-        <is>
-          <t>TR40VA004</t>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>FX-SC8D005M1-0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Mantenimiento de software inicial de 1 año para el controlador de supervisión FX80 con capacidad de 5–9 dispositivos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion bug mejoras modulo tareas, envio de notificacion al correo, correccion bug al generar puntos de control
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="TAB CONT 01" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Supervisor" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TAB CONT 02" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Supervisor" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -500,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +532,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CFP2</t>
+          <t>URGENCIAS FUNDACIÓN CARDIO INFANTIL</t>
         </is>
       </c>
     </row>
@@ -559,16 +560,16 @@
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -583,16 +584,16 @@
     </row>
     <row r="5">
       <c r="C5" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -610,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -711,7 +712,7 @@
     <row r="9">
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>VENT 01</t>
+          <t>BAF01</t>
         </is>
       </c>
       <c r="K9" s="3" t="inlineStr">
@@ -721,23 +722,26 @@
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>F4-CGM04060</t>
+          <t>F4-CGM09090-0</t>
         </is>
       </c>
       <c r="M9" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" s="8" t="n">
         <v>3</v>
-      </c>
-      <c r="N9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P9" s="8" t="n">
-        <v>2</v>
       </c>
       <c r="Q9" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R9" s="9" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -746,7 +750,7 @@
       </c>
       <c r="B10" s="10" t="inlineStr">
         <is>
-          <t>CONTROL DE PRESIÓN DIFERENCIAL SWITCH</t>
+          <t>Estado</t>
         </is>
       </c>
       <c r="D10" s="11" t="n">
@@ -764,15 +768,18 @@
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>FX-PCX4711-0</t>
+          <t>F4-XPM09090-0</t>
         </is>
       </c>
       <c r="M10" s="8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N10" s="8" t="n">
         <v>2</v>
       </c>
+      <c r="O10" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="P10" s="8" t="n">
         <v>3</v>
       </c>
@@ -780,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="R10" s="9" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -789,15 +796,15 @@
       </c>
       <c r="B11" s="10" t="inlineStr">
         <is>
-          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
-        </is>
-      </c>
-      <c r="C11" s="11" t="n">
+          <t>ON-Off</t>
+        </is>
+      </c>
+      <c r="F11" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="12" t="inlineStr">
         <is>
-          <t>AQD-BBBE - SENVA</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
@@ -807,15 +814,15 @@
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>CONDUCTO DE TEMPERATURA DE HUMEDAD</t>
-        </is>
-      </c>
-      <c r="C12" s="11" t="n">
-        <v>2</v>
+          <t>FallaUV</t>
+        </is>
+      </c>
+      <c r="F12" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="H12" s="12" t="inlineStr">
         <is>
-          <t>HT1D - SENVA</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
@@ -824,39 +831,28 @@
         </is>
       </c>
       <c r="M12" s="3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q12" s="3" t="n">
         <v>8</v>
       </c>
       <c r="R12" s="9" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B13" s="10" t="inlineStr">
-        <is>
-          <t>START/STOP VENT 01</t>
-        </is>
-      </c>
-      <c r="F13" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12" t="inlineStr">
-        <is>
-          <t>CKIT-VMD1B-C24A - VERIS</t>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Chiller01</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
@@ -868,28 +864,28 @@
         <v>7</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P13" s="3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R13" s="9" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B14" s="10" t="inlineStr">
         <is>
-          <t>PARO DE EMERGANCIA</t>
+          <t>Alarma</t>
         </is>
       </c>
       <c r="D14" s="11" t="n">
@@ -906,64 +902,75 @@
         </is>
       </c>
       <c r="M14" s="4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N14" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O14" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="P14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P14" s="4" t="n">
-        <v>3</v>
-      </c>
       <c r="Q14" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R14" s="9" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="6" t="inlineStr">
-        <is>
-          <t>VENT 02</t>
+      <c r="A15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" s="10" t="inlineStr">
         <is>
-          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
-        </is>
-      </c>
-      <c r="C16" s="11" t="n">
+          <t>ReqBomba</t>
+        </is>
+      </c>
+      <c r="D16" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
-          <t>AQD-BBBE - SENVA</t>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" s="10" t="inlineStr">
         <is>
-          <t>CONTROL DE PRESIÓN DIFERENCIAL SWITCH</t>
-        </is>
-      </c>
-      <c r="D17" s="11" t="n">
+          <t>ON-OFF</t>
+        </is>
+      </c>
+      <c r="F17" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H17" s="12" t="inlineStr">
         <is>
-          <t>P74FA-1C - JOHNSON CONTROLS</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
@@ -978,20 +985,9 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="10" t="inlineStr">
-        <is>
-          <t>CONDUCTO DE TEMPERATURA DE HUMEDAD</t>
-        </is>
-      </c>
-      <c r="C18" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="H18" s="12" t="inlineStr">
-        <is>
-          <t>HT1D - SENVA</t>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>BAF02</t>
         </is>
       </c>
       <c r="K18" s="13" t="n">
@@ -1005,35 +1001,247 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19" s="10" t="inlineStr">
         <is>
-          <t>START/STOP VENT 02</t>
-        </is>
-      </c>
-      <c r="F19" s="11" t="n">
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H19" s="12" t="inlineStr">
         <is>
-          <t>CKIT-VMD1B-C24A - VERIS</t>
+          <t>P74FA-1C - JOHNSON CONTROLS</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>ON-Off</t>
+        </is>
+      </c>
+      <c r="F20" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="F21" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>VE07</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D23" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="12" t="inlineStr">
+        <is>
+          <t>AFS-262 - CLEVELAND CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>EstadoLampUV</t>
+        </is>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="F25" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>FallaVE</t>
+        </is>
+      </c>
+      <c r="F26" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B20" s="10" t="inlineStr">
-        <is>
-          <t>PARO DE EMERGANCIA</t>
-        </is>
-      </c>
-      <c r="D20" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="12" t="inlineStr">
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>DPT Zona</t>
+        </is>
+      </c>
+      <c r="C27" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12" t="inlineStr">
+        <is>
+          <t>DP150MR1-SA - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>VE08</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>DPT Zona</t>
+        </is>
+      </c>
+      <c r="C29" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="12" t="inlineStr">
+        <is>
+          <t>DP150MR1-SA - JOHNSON CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D30" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12" t="inlineStr">
+        <is>
+          <t>AFS-262 - CLEVELAND CONTROLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>FallaVE</t>
+        </is>
+      </c>
+      <c r="F31" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" s="10" t="inlineStr">
+        <is>
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="F32" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>EstadoLampUV</t>
+        </is>
+      </c>
+      <c r="D33" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="12" t="inlineStr">
         <is>
           <t>BI - T&amp;S</t>
         </is>
@@ -1045,6 +1253,1965 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R89"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="5" customWidth="1" min="3" max="3"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="2" customWidth="1" min="9" max="9"/>
+    <col width="2" customWidth="1" min="10" max="10"/>
+    <col width="5" customWidth="1" min="11" max="11"/>
+    <col width="32" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>PROYECTO</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>URGENCIAS FUNDACIÓN CARDIO INFANTIL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SISTEMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TAB CONT 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SOLUCIÓN</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>JCI FACILITY EXPLORER</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>&lt;==</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCIÓN</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>NOTAS / TIPO DE SENSOR / ACTUADOR</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>CONTROLADOR / EXPANSIÓN</t>
+        </is>
+      </c>
+      <c r="M8" s="5" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="O8" s="5" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="P8" s="5" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="Q8" s="5" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="R8" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>VentSum1-19</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>F4-CGM09090-0</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>FX-PCX3721-0</t>
+        </is>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="R10" s="9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L11" s="7" t="inlineStr">
+        <is>
+          <t>F4-XPM09090-0</t>
+        </is>
+      </c>
+      <c r="M11" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N11" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O11" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P11" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L12" s="7" t="inlineStr">
+        <is>
+          <t>F4-XPM09090-0</t>
+        </is>
+      </c>
+      <c r="M12" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N12" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R12" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L13" s="7" t="inlineStr">
+        <is>
+          <t>F4-XPM09090-0</t>
+        </is>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L14" s="7" t="inlineStr">
+        <is>
+          <t>F4-XPM09090-0</t>
+        </is>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R14" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L15" s="7" t="inlineStr">
+        <is>
+          <t>F4-XPM04060-0</t>
+        </is>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R15" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L16" s="7" t="inlineStr">
+        <is>
+          <t>F4-XPM04060-0</t>
+        </is>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R16" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L18" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O18" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="R18" s="9" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L19" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="R19" s="9" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M20" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="N20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="P20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="R20" s="9" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F22" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D23" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K23" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L23" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K24" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L24" s="13" t="inlineStr">
+        <is>
+          <t>TR100VA004</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F25" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D26" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F28" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D29" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D30" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F31" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B32" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D32" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D33" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B34" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F34" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B35" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B36" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F37" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B38" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D38" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D39" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B40" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F40" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="B41" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D41" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D42" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B43" s="10" t="inlineStr">
+        <is>
+          <t>ON-OFF</t>
+        </is>
+      </c>
+      <c r="F43" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>ON-OFF</t>
+        </is>
+      </c>
+      <c r="F44" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="B45" s="10" t="inlineStr">
+        <is>
+          <t>ON-OFF</t>
+        </is>
+      </c>
+      <c r="F45" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="B46" s="10" t="inlineStr">
+        <is>
+          <t>ON-OFF</t>
+        </is>
+      </c>
+      <c r="F46" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="B47" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F47" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="B48" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F48" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="B49" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F49" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="B50" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F50" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="B51" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F51" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="B52" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F52" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="B53" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F53" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="B54" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F54" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="B55" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F55" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="B56" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F56" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F57" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="B58" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F58" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="B59" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D59" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="B60" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F60" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="B61" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D61" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="n">
+        <v>53</v>
+      </c>
+      <c r="B62" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F62" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="B63" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F63" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="B64" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D64" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="B65" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D65" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="B66" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F66" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="B67" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F67" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B68" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D68" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="B69" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D69" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B70" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F70" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="n">
+        <v>62</v>
+      </c>
+      <c r="B71" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D71" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="B72" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D72" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="B73" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F73" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="B74" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F74" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="B75" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D75" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="B76" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D76" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="B77" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F77" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="B78" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F78" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="B79" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F79" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B80" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D80" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B81" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D81" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B82" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F82" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H82" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="n">
+        <v>74</v>
+      </c>
+      <c r="B83" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F83" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H83" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="n">
+        <v>75</v>
+      </c>
+      <c r="B84" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D84" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="B85" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D85" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="B86" s="10" t="inlineStr">
+        <is>
+          <t>PUNTO DIGITAL DE SALIDA</t>
+        </is>
+      </c>
+      <c r="F86" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" s="12" t="inlineStr">
+        <is>
+          <t>BO - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="n">
+        <v>78</v>
+      </c>
+      <c r="B87" s="10" t="inlineStr">
+        <is>
+          <t>Falla</t>
+        </is>
+      </c>
+      <c r="F87" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" s="12" t="inlineStr">
+        <is>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="B88" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D88" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="B89" s="10" t="inlineStr">
+        <is>
+          <t>EstadoFil</t>
+        </is>
+      </c>
+      <c r="D89" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
mejora al encontrar expansiones para calcular puntos.
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -501,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,13 +563,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -587,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>
@@ -611,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>4</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>5</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -750,15 +750,15 @@
       </c>
       <c r="B10" s="10" t="inlineStr">
         <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="D10" s="11" t="n">
+          <t>ON-Off</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="12" t="inlineStr">
         <is>
-          <t>P74FA-1C - JOHNSON CONTROLS</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
       <c r="K10" s="3" t="inlineStr">
@@ -768,26 +768,23 @@
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM09090-0</t>
+          <t>F4-XPM04060-0</t>
         </is>
       </c>
       <c r="M10" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" s="8" t="n">
         <v>2</v>
-      </c>
-      <c r="O10" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P10" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="Q10" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R10" s="9" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -796,7 +793,7 @@
       </c>
       <c r="B11" s="10" t="inlineStr">
         <is>
-          <t>ON-Off</t>
+          <t>FallaUV</t>
         </is>
       </c>
       <c r="F11" s="11" t="n">
@@ -809,50 +806,50 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>Chiller01</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N12" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="10" t="inlineStr">
-        <is>
-          <t>FallaUV</t>
-        </is>
-      </c>
-      <c r="F12" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12" t="inlineStr">
-        <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
-        </is>
-      </c>
-      <c r="L12" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
-        </is>
-      </c>
-      <c r="M12" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="N12" s="3" t="n">
-        <v>4</v>
-      </c>
       <c r="O12" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="3" t="n">
         <v>8</v>
       </c>
       <c r="R12" s="9" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="6" t="inlineStr">
-        <is>
-          <t>Chiller01</t>
+      <c r="A13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
@@ -861,31 +858,31 @@
         </is>
       </c>
       <c r="M13" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P13" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q13" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R13" s="9" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="10" t="inlineStr">
         <is>
-          <t>Alarma</t>
+          <t>Estado</t>
         </is>
       </c>
       <c r="D14" s="11" t="n">
@@ -902,31 +899,31 @@
         </is>
       </c>
       <c r="M14" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N14" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O14" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P14" s="4" t="n">
         <v>0</v>
       </c>
       <c r="Q14" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R14" s="9" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="10" t="inlineStr">
         <is>
-          <t>Estado</t>
+          <t>ReqBomba</t>
         </is>
       </c>
       <c r="D15" s="11" t="n">
@@ -940,54 +937,54 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="10" t="inlineStr">
         <is>
-          <t>ReqBomba</t>
-        </is>
-      </c>
-      <c r="D16" s="11" t="n">
+          <t>ON-OFF</t>
+        </is>
+      </c>
+      <c r="F16" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
-          <t>BI - T&amp;S</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" s="10" t="inlineStr">
-        <is>
-          <t>ON-OFF</t>
-        </is>
-      </c>
-      <c r="F17" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="12" t="inlineStr">
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>BAF02</t>
+        </is>
+      </c>
+      <c r="K17" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L17" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>ON-Off sdsdsd</t>
+        </is>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
         <is>
           <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
-        </is>
-      </c>
-      <c r="K17" s="1" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="L17" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="6" t="inlineStr">
-        <is>
-          <t>BAF02</t>
         </is>
       </c>
       <c r="K18" s="13" t="n">
@@ -1001,140 +998,129 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="10" t="inlineStr">
         <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="D19" s="11" t="n">
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="F19" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H19" s="12" t="inlineStr">
         <is>
-          <t>P74FA-1C - JOHNSON CONTROLS</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B20" s="10" t="inlineStr">
-        <is>
-          <t>ON-Off</t>
-        </is>
-      </c>
-      <c r="F20" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="12" t="inlineStr">
-        <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>VE07</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" s="10" t="inlineStr">
         <is>
-          <t>Alarma</t>
-        </is>
-      </c>
-      <c r="F21" s="11" t="n">
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H21" s="12" t="inlineStr">
         <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+          <t>AFS-262 - CLEVELAND CONTROLS</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="6" t="inlineStr">
-        <is>
-          <t>VE07</t>
+      <c r="A22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>EstadoLampUV</t>
+        </is>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" s="10" t="inlineStr">
         <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="D23" s="11" t="n">
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="F23" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H23" s="12" t="inlineStr">
         <is>
-          <t>AFS-262 - CLEVELAND CONTROLS</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B24" s="10" t="inlineStr">
         <is>
-          <t>EstadoLampUV</t>
-        </is>
-      </c>
-      <c r="D24" s="11" t="n">
+          <t>FallaVE</t>
+        </is>
+      </c>
+      <c r="F24" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H24" s="12" t="inlineStr">
         <is>
-          <t>BI - T&amp;S</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" s="10" t="inlineStr">
         <is>
-          <t>Alarma</t>
-        </is>
-      </c>
-      <c r="F25" s="11" t="n">
+          <t>DPT Zona</t>
+        </is>
+      </c>
+      <c r="C25" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H25" s="12" t="inlineStr">
         <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+          <t>DP150MR1-SA - JOHNSON CONTROLS</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B26" s="10" t="inlineStr">
-        <is>
-          <t>FallaVE</t>
-        </is>
-      </c>
-      <c r="F26" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="12" t="inlineStr">
-        <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>VE08</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B27" s="10" t="inlineStr">
         <is>
@@ -1151,97 +1137,72 @@
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="6" t="inlineStr">
-        <is>
-          <t>VE08</t>
+      <c r="A28" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D28" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="12" t="inlineStr">
+        <is>
+          <t>AFS-262 - CLEVELAND CONTROLS</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B29" s="10" t="inlineStr">
         <is>
-          <t>DPT Zona</t>
-        </is>
-      </c>
-      <c r="C29" s="11" t="n">
+          <t>FallaVE</t>
+        </is>
+      </c>
+      <c r="F29" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H29" s="12" t="inlineStr">
         <is>
-          <t>DP150MR1-SA - JOHNSON CONTROLS</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B30" s="10" t="inlineStr">
         <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="D30" s="11" t="n">
+          <t>Alarma</t>
+        </is>
+      </c>
+      <c r="F30" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H30" s="12" t="inlineStr">
         <is>
-          <t>AFS-262 - CLEVELAND CONTROLS</t>
+          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B31" s="10" t="inlineStr">
         <is>
-          <t>FallaVE</t>
-        </is>
-      </c>
-      <c r="F31" s="11" t="n">
+          <t>EstadoLampUV</t>
+        </is>
+      </c>
+      <c r="D31" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="12" t="inlineStr">
-        <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B32" s="10" t="inlineStr">
-        <is>
-          <t>Alarma</t>
-        </is>
-      </c>
-      <c r="F32" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="12" t="inlineStr">
-        <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B33" s="10" t="inlineStr">
-        <is>
-          <t>EstadoLampUV</t>
-        </is>
-      </c>
-      <c r="D33" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" s="12" t="inlineStr">
         <is>
           <t>BI - T&amp;S</t>
         </is>
@@ -1313,20 +1274,20 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>JCI FACILITY EXPLORER</t>
+          <t>JCI METASYS</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -1368,13 +1329,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -1479,7 +1440,7 @@
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>F4-CGM09090-0</t>
+          <t>M4-CGM09090-0</t>
         </is>
       </c>
       <c r="M9" s="8" t="n">
@@ -1525,14 +1486,23 @@
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>FX-PCX3721-0</t>
-        </is>
+          <t>M4-XPM04060-0</t>
+        </is>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>3</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="P10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="8" t="n">
+        <v>4</v>
       </c>
       <c r="R10" s="9" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -1559,26 +1529,23 @@
       </c>
       <c r="L11" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM09090-0</t>
+          <t>M4-XPM04060-0</t>
         </is>
       </c>
       <c r="M11" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" s="8" t="n">
         <v>2</v>
-      </c>
-      <c r="O11" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P11" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="Q11" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R11" s="9" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1605,26 +1572,23 @@
       </c>
       <c r="L12" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM09090-0</t>
+          <t>M4-XPM04060-0</t>
         </is>
       </c>
       <c r="M12" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="8" t="n">
         <v>2</v>
-      </c>
-      <c r="O12" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P12" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="Q12" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R12" s="9" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -1651,26 +1615,23 @@
       </c>
       <c r="L13" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM09090-0</t>
+          <t>M4-XPM04060-0</t>
         </is>
       </c>
       <c r="M13" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="8" t="n">
         <v>2</v>
-      </c>
-      <c r="O13" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P13" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="Q13" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R13" s="9" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1697,26 +1658,23 @@
       </c>
       <c r="L14" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM09090-0</t>
+          <t>M4-XPM04060-0</t>
         </is>
       </c>
       <c r="M14" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N14" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="8" t="n">
         <v>2</v>
-      </c>
-      <c r="O14" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="P14" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="Q14" s="8" t="n">
         <v>4</v>
       </c>
       <c r="R14" s="9" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1743,7 +1701,7 @@
       </c>
       <c r="L15" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM04060-0</t>
+          <t>M4-XPM04060-0</t>
         </is>
       </c>
       <c r="M15" s="8" t="n">
@@ -1786,7 +1744,7 @@
       </c>
       <c r="L16" s="7" t="inlineStr">
         <is>
-          <t>F4-XPM04060-0</t>
+          <t>M4-XPM04060-0</t>
         </is>
       </c>
       <c r="M16" s="8" t="n">
@@ -1822,6 +1780,31 @@
           <t>BI - T&amp;S</t>
         </is>
       </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="L17" s="7" t="inlineStr">
+        <is>
+          <t>M4-XPM04060-0</t>
+        </is>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R17" s="9" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
@@ -1840,29 +1823,6 @@
           <t>BI - T&amp;S</t>
         </is>
       </c>
-      <c r="L18" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
-        </is>
-      </c>
-      <c r="M18" s="3" t="n">
-        <v>41</v>
-      </c>
-      <c r="N18" s="3" t="n">
-        <v>28</v>
-      </c>
-      <c r="O18" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="P18" s="3" t="n">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="3" t="n">
-        <v>28</v>
-      </c>
-      <c r="R18" s="9" t="n">
-        <v>126</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="n">
@@ -1883,26 +1843,26 @@
       </c>
       <c r="L19" s="1" t="inlineStr">
         <is>
-          <t>PUNTOS PROYECTADOS</t>
+          <t>PUNTOS DISPONIBLES EN CONTROLES</t>
         </is>
       </c>
       <c r="M19" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="N19" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="N19" s="3" t="n">
-        <v>28</v>
-      </c>
       <c r="O19" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P19" s="3" t="n">
         <v>19</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="R19" s="9" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20">
@@ -1924,26 +1884,26 @@
       </c>
       <c r="L20" s="1" t="inlineStr">
         <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M20" s="4" t="n">
-        <v>31</v>
-      </c>
-      <c r="N20" s="4" t="n">
+          <t>PUNTOS PROYECTADOS</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="N20" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O20" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O20" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="P20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="4" t="n">
-        <v>5</v>
+      <c r="P20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="3" t="n">
+        <v>23</v>
       </c>
       <c r="R20" s="9" t="n">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
@@ -1963,6 +1923,29 @@
           <t>BI - T&amp;S</t>
         </is>
       </c>
+      <c r="L21" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M21" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="R21" s="9" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
@@ -1999,16 +1982,6 @@
           <t>BI - T&amp;S</t>
         </is>
       </c>
-      <c r="K23" s="1" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="L23" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
@@ -2027,12 +2000,14 @@
           <t>BI - T&amp;S</t>
         </is>
       </c>
-      <c r="K24" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="L24" s="13" t="inlineStr">
-        <is>
-          <t>TR100VA004</t>
+      <c r="K24" s="1" t="inlineStr">
+        <is>
+          <t>CANT</t>
+        </is>
+      </c>
+      <c r="L24" s="1" t="inlineStr">
+        <is>
+          <t>ACCESORIO</t>
         </is>
       </c>
     </row>
@@ -2051,6 +2026,14 @@
       <c r="H25" s="12" t="inlineStr">
         <is>
           <t>BO - T&amp;S</t>
+        </is>
+      </c>
+      <c r="K25" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" s="13" t="inlineStr">
+        <is>
+          <t>TR100VA004</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
correccion de bug al subir documentos y archivar proyecto
</commit_message>
<xml_diff>
--- a/tsinc/static/points/Points.xlsx
+++ b/tsinc/static/points/Points.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="TAB CONT 01" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Supervisor" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -99,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -131,9 +130,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +527,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CFP2</t>
+          <t>PRUEBA</t>
         </is>
       </c>
     </row>
@@ -562,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0</v>
@@ -586,13 +582,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -610,13 +606,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -711,7 +707,7 @@
     <row r="9">
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>VENT 01</t>
+          <t>EQUIPO</t>
         </is>
       </c>
       <c r="K9" s="3" t="inlineStr">
@@ -746,7 +742,7 @@
       </c>
       <c r="B10" s="10" t="inlineStr">
         <is>
-          <t>Estado2</t>
+          <t xml:space="preserve">ESTADO </t>
         </is>
       </c>
       <c r="D10" s="11" t="n">
@@ -754,7 +750,7 @@
       </c>
       <c r="H10" s="12" t="inlineStr">
         <is>
-          <t>P74FA-1C - JOHNSON CONTROLS</t>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
       <c r="K10" s="3" t="inlineStr">
@@ -764,14 +760,14 @@
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>FX-PCX1711</t>
+          <t>FX-PCX3721-0</t>
         </is>
       </c>
       <c r="N10" s="8" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="R10" s="9" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -780,15 +776,15 @@
       </c>
       <c r="B11" s="10" t="inlineStr">
         <is>
-          <t>START/STOP VENT 01</t>
-        </is>
-      </c>
-      <c r="F11" s="11" t="n">
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D11" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="12" t="inlineStr">
         <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
@@ -798,7 +794,7 @@
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>PARO DE EMERGANCIA</t>
+          <t xml:space="preserve">ESTADO </t>
         </is>
       </c>
       <c r="D12" s="11" t="n">
@@ -818,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="O12" s="3" t="n">
         <v>0</v>
@@ -830,7 +826,7 @@
         <v>4</v>
       </c>
       <c r="R12" s="9" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -839,7 +835,7 @@
       </c>
       <c r="B13" s="10" t="inlineStr">
         <is>
-          <t>PARO DE EMERGANCIA</t>
+          <t xml:space="preserve">ESTADO </t>
         </is>
       </c>
       <c r="D13" s="11" t="n">
@@ -856,61 +852,72 @@
         </is>
       </c>
       <c r="M13" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="O13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="O13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3" t="n">
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>PUNTOS SOBRANTES</t>
+        </is>
+      </c>
+      <c r="M14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4" t="n">
         <v>2</v>
-      </c>
-      <c r="Q13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="6" t="inlineStr">
-        <is>
-          <t>VENT 02</t>
-        </is>
-      </c>
-      <c r="L14" s="1" t="inlineStr">
-        <is>
-          <t>PUNTOS SOBRANTES</t>
-        </is>
-      </c>
-      <c r="M14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="Q14" s="4" t="n">
         <v>4</v>
       </c>
       <c r="R14" s="9" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B15" s="10" t="inlineStr">
         <is>
-          <t>Estado3</t>
+          <t xml:space="preserve">ESTADO </t>
         </is>
       </c>
       <c r="D15" s="11" t="n">
@@ -918,35 +925,35 @@
       </c>
       <c r="H15" s="12" t="inlineStr">
         <is>
-          <t>P74FA-1C - JOHNSON CONTROLS</t>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B16" s="10" t="inlineStr">
         <is>
-          <t>START/STOP VENT 02</t>
-        </is>
-      </c>
-      <c r="F16" s="11" t="n">
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D16" s="11" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="12" t="inlineStr">
         <is>
-          <t>VMD1B-F24A-02A - VERIS INDUSTRIES</t>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B17" s="10" t="inlineStr">
         <is>
-          <t>PARO DE EMERGANCIA</t>
+          <t xml:space="preserve">ESTADO </t>
         </is>
       </c>
       <c r="D17" s="11" t="n">
@@ -970,11 +977,11 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B18" s="10" t="inlineStr">
         <is>
-          <t>PARO DE EMERGANCIA</t>
+          <t xml:space="preserve">ESTADO </t>
         </is>
       </c>
       <c r="D18" s="11" t="n">
@@ -994,117 +1001,129 @@
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B2:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="100" customWidth="1" min="3" max="3"/>
-    <col width="32" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>SUPERVISOR</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="F2" s="5" t="inlineStr">
-        <is>
-          <t>CANT</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
-        <is>
-          <t>ACCESORIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="14" t="inlineStr">
-        <is>
-          <t>FX80</t>
-        </is>
-      </c>
-      <c r="C3" s="14" t="inlineStr">
-        <is>
-          <t>MODULO SUPERVISOR JC FX80</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14" t="inlineStr">
-        <is>
-          <t>TR40VA004</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>LICENCIA</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>FX-SC8BASE-0</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Controlador de supervisión FX80 y tarjeta micro Secure Digital (SD)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>FX-SC8CL005-0</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Licencia de dispositivo central del controlador de supervisión FX80; 5 dispositivos de campo; 250 puntos</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>FX-SC8D005M1-0</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Mantenimiento de software inicial de 1 año para el controlador de supervisión FX80 con capacidad de 5–9 dispositivos</t>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D23" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESTADO </t>
+        </is>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12" t="inlineStr">
+        <is>
+          <t>BI - T&amp;S</t>
         </is>
       </c>
     </row>

</xml_diff>